<commit_message>
TP#15401 Canada Express International fixes
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="230">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -680,9 +680,6 @@
   </si>
   <si>
     <t>IP-1012</t>
-  </si>
-  <si>
-    <t>INTERNATIONAL_TRAFFIC_IN_ARMS_REGULATIONS</t>
   </si>
   <si>
     <t>IPF-1002</t>
@@ -1211,16 +1208,16 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
@@ -1546,9 +1543,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:DT15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BW1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BY19" sqref="BY19"/>
+      <selection pane="bottomLeft" activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2379,7 +2376,7 @@
       <c r="A3" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -2637,7 +2634,7 @@
       <c r="A4" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="59"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="18" t="s">
         <v>119</v>
       </c>
@@ -2921,7 +2918,7 @@
       <c r="A5" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="59"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="18" t="s">
         <v>119</v>
       </c>
@@ -3157,7 +3154,7 @@
       <c r="A6" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="18" t="s">
         <v>119</v>
       </c>
@@ -3407,7 +3404,7 @@
       <c r="A7" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="18" t="s">
         <v>119</v>
       </c>
@@ -3667,7 +3664,7 @@
       <c r="A8" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="30" t="s">
         <v>119</v>
       </c>
@@ -3927,7 +3924,7 @@
       <c r="A9" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="18" t="s">
         <v>119</v>
       </c>
@@ -4185,7 +4182,7 @@
       <c r="A10" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="18" t="s">
         <v>119</v>
       </c>
@@ -4449,7 +4446,7 @@
       <c r="A11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="59"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="18" t="s">
         <v>119</v>
       </c>
@@ -4715,7 +4712,7 @@
       <c r="A12" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="18" t="s">
         <v>119</v>
       </c>
@@ -4798,9 +4795,7 @@
       <c r="AD12" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AE12" s="38" t="s">
-        <v>216</v>
-      </c>
+      <c r="AE12" s="38"/>
       <c r="AF12" s="20"/>
       <c r="AG12" s="20" t="s">
         <v>138</v>
@@ -4969,12 +4964,12 @@
       <c r="A13" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="59"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="18" t="s">
         <v>119</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
@@ -5017,7 +5012,7 @@
         <v>132</v>
       </c>
       <c r="S13" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T13" s="20" t="s">
         <v>133</v>
@@ -5052,9 +5047,7 @@
       <c r="AD13" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AE13" s="38" t="s">
-        <v>216</v>
-      </c>
+      <c r="AE13" s="38"/>
       <c r="AF13" s="20"/>
       <c r="AG13" s="20" t="s">
         <v>138</v>
@@ -5235,12 +5228,12 @@
       <c r="A14" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="59"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="18" t="s">
         <v>119</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20" t="s">
@@ -5250,7 +5243,7 @@
         <v>123</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>173</v>
@@ -5283,7 +5276,7 @@
         <v>132</v>
       </c>
       <c r="S14" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T14" s="20" t="s">
         <v>133</v>
@@ -5295,13 +5288,13 @@
         <v>128</v>
       </c>
       <c r="W14" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X14" s="20" t="s">
         <v>186</v>
       </c>
       <c r="Y14" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z14" s="20" t="s">
         <v>137</v>
@@ -5319,7 +5312,7 @@
         <v>132</v>
       </c>
       <c r="AE14" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF14" s="20"/>
       <c r="AG14" s="20" t="s">
@@ -5407,7 +5400,7 @@
       <c r="BK14" s="20"/>
       <c r="BL14" s="20"/>
       <c r="BM14" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="BN14" s="20">
         <v>1</v>
@@ -5434,7 +5427,7 @@
         <v>20</v>
       </c>
       <c r="BV14" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BW14" s="20" t="s">
         <v>154</v>
@@ -5444,11 +5437,11 @@
       </c>
       <c r="BY14" s="20"/>
       <c r="BZ14" s="20"/>
-      <c r="CA14" s="61" t="s">
+      <c r="CA14" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="CB14" s="60" t="s">
         <v>229</v>
-      </c>
-      <c r="CB14" s="62" t="s">
-        <v>230</v>
       </c>
       <c r="CC14" s="20"/>
       <c r="CD14" s="20" t="s">
@@ -5458,7 +5451,7 @@
       <c r="CF14" s="20"/>
       <c r="CG14" s="20"/>
       <c r="CH14" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CI14" s="27" t="s">
         <v>164</v>
@@ -5476,7 +5469,7 @@
         <v>128</v>
       </c>
       <c r="CN14" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CO14" s="27" t="s">
         <v>186</v>
@@ -5523,12 +5516,12 @@
       <c r="A15" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="60"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="42" t="s">
         <v>119</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E15" s="44"/>
       <c r="F15" s="44" t="s">
@@ -5571,7 +5564,7 @@
         <v>132</v>
       </c>
       <c r="S15" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T15" s="44" t="s">
         <v>133</v>
@@ -5583,13 +5576,13 @@
         <v>128</v>
       </c>
       <c r="W15" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X15" s="44" t="s">
         <v>186</v>
       </c>
       <c r="Y15" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z15" s="44" t="s">
         <v>137</v>
@@ -5607,7 +5600,7 @@
         <v>132</v>
       </c>
       <c r="AE15" s="47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF15" s="44"/>
       <c r="AG15" s="44" t="s">
@@ -5695,7 +5688,7 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
       <c r="BM15" s="44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="BN15" s="44">
         <v>1</v>
@@ -5722,7 +5715,7 @@
         <v>20</v>
       </c>
       <c r="BV15" s="44" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BW15" s="44" t="s">
         <v>154</v>
@@ -5732,11 +5725,11 @@
       </c>
       <c r="BY15" s="44"/>
       <c r="BZ15" s="44"/>
-      <c r="CA15" s="61" t="s">
+      <c r="CA15" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="CB15" s="60" t="s">
         <v>229</v>
-      </c>
-      <c r="CB15" s="62" t="s">
-        <v>230</v>
       </c>
       <c r="CC15" s="44"/>
       <c r="CD15" s="44" t="s">
@@ -5746,7 +5739,7 @@
       <c r="CF15" s="44"/>
       <c r="CG15" s="44"/>
       <c r="CH15" s="49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CI15" s="49" t="s">
         <v>164</v>
@@ -5764,7 +5757,7 @@
         <v>128</v>
       </c>
       <c r="CN15" s="49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CO15" s="49" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
TP#15879 Update integration tests to use hazmat
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Shipworks2\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="231">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>PASSPORT</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL_TRAFFIC_IN_ARMS_REGULATIONS</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1548,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA32" sqref="AA32"/>
+      <selection pane="bottomLeft" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4795,7 +4798,9 @@
       <c r="AD12" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AE12" s="38"/>
+      <c r="AE12" s="38" t="s">
+        <v>230</v>
+      </c>
       <c r="AF12" s="20"/>
       <c r="AG12" s="20" t="s">
         <v>138</v>
@@ -5047,7 +5052,9 @@
       <c r="AD13" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AE13" s="38"/>
+      <c r="AE13" s="38" t="s">
+        <v>230</v>
+      </c>
       <c r="AF13" s="20"/>
       <c r="AG13" s="20" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
TP#20088: Updated for spreadsheets.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Intl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,13 +21,13 @@
     <definedName name="_lu2" localSheetId="0">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="236">
   <si>
     <t>FEDEX BUSINESS</t>
   </si>
@@ -723,12 +723,24 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedShipment.CustomsClearanceDetail.ImporterOfRecord.Contact</t>
+  </si>
+  <si>
+    <t>Importer Name</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedShipment.SpecialServicesRequested4</t>
+  </si>
+  <si>
+    <t>ProcessShipmentRequest.RequestedShipment.SpecialServicesRequested3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1827,12 +1839,6 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1841,6 +1847,12 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="364">
@@ -2312,23 +2324,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2364,23 +2359,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2559,10 +2537,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JS15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CE1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="CG1" sqref="CG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2645,11 +2623,12 @@
     <col min="119" max="120" width="51.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="121" max="122" width="51.5703125" style="2" customWidth="1"/>
     <col min="123" max="124" width="70" style="2" bestFit="1" customWidth="1"/>
-    <col min="125" max="16384" width="9.140625" style="2"/>
+    <col min="125" max="125" width="60.5703125" style="2" customWidth="1"/>
+    <col min="126" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:279" s="17" customFormat="1" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>231</v>
       </c>
       <c r="B1" s="22"/>
@@ -2894,10 +2873,10 @@
         <v>210</v>
       </c>
       <c r="CE1" s="23" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="CF1" s="23" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="CG1" s="23" t="s">
         <v>211</v>
@@ -3018,6 +2997,9 @@
       </c>
       <c r="DT1" s="25" t="s">
         <v>214</v>
+      </c>
+      <c r="DU1" s="25" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:279" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3387,12 +3369,15 @@
       <c r="DT2" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="DU2" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="79" t="b">
+    <row r="3" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="52" t="s">
@@ -3643,12 +3628,15 @@
       <c r="DR3" s="40"/>
       <c r="DS3" s="40"/>
       <c r="DT3" s="45"/>
+      <c r="DU3" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="4" spans="1:279" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="79" t="b">
+    <row r="4" spans="1:279" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="76"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="53" t="s">
         <v>35</v>
       </c>
@@ -3927,12 +3915,15 @@
       <c r="DR4" s="28"/>
       <c r="DS4" s="28"/>
       <c r="DT4" s="31"/>
+      <c r="DU4" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="5" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="79" t="b">
+    <row r="5" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="76"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="53" t="s">
         <v>35</v>
       </c>
@@ -4163,12 +4154,15 @@
       <c r="DR5" s="28"/>
       <c r="DS5" s="28"/>
       <c r="DT5" s="31"/>
+      <c r="DU5" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="6" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="79" t="b">
+    <row r="6" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="53" t="s">
         <v>35</v>
       </c>
@@ -4411,12 +4405,15 @@
       <c r="DR6" s="28"/>
       <c r="DS6" s="28"/>
       <c r="DT6" s="31"/>
+      <c r="DU6" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="7" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="79" t="b">
+    <row r="7" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="76"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="53" t="s">
         <v>35</v>
       </c>
@@ -4671,12 +4668,15 @@
       <c r="DR7" s="28"/>
       <c r="DS7" s="28"/>
       <c r="DT7" s="31"/>
+      <c r="DU7" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="8" spans="1:279" s="14" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="79" t="b">
+    <row r="8" spans="1:279" s="14" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="54" t="s">
         <v>35</v>
       </c>
@@ -4931,12 +4931,15 @@
       <c r="DR8" s="32"/>
       <c r="DS8" s="32"/>
       <c r="DT8" s="35"/>
+      <c r="DU8" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="9" spans="1:279" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="79" t="b">
+    <row r="9" spans="1:279" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="76"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="53" t="s">
         <v>35</v>
       </c>
@@ -5189,12 +5192,15 @@
       <c r="DR9" s="28"/>
       <c r="DS9" s="28"/>
       <c r="DT9" s="31"/>
+      <c r="DU9" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="10" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="79" t="b">
+    <row r="10" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="76"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="53" t="s">
         <v>35</v>
       </c>
@@ -5453,12 +5459,15 @@
       <c r="DR10" s="28"/>
       <c r="DS10" s="28"/>
       <c r="DT10" s="31"/>
+      <c r="DU10" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="11" spans="1:279" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="79" t="b">
+    <row r="11" spans="1:279" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="76"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="53" t="s">
         <v>35</v>
       </c>
@@ -5725,12 +5734,15 @@
       </c>
       <c r="DS11" s="28"/>
       <c r="DT11" s="31"/>
+      <c r="DU11" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="12" spans="1:279" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="79" t="b">
+    <row r="12" spans="1:279" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="76"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="53" t="s">
         <v>35</v>
       </c>
@@ -5979,12 +5991,15 @@
       <c r="DR12" s="32"/>
       <c r="DS12" s="28"/>
       <c r="DT12" s="31"/>
+      <c r="DU12" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="13" spans="1:279" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="79" t="b">
+    <row r="13" spans="1:279" s="15" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="76"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="53" t="s">
         <v>35</v>
       </c>
@@ -6243,12 +6258,15 @@
       <c r="DR13" s="28"/>
       <c r="DS13" s="28"/>
       <c r="DT13" s="31"/>
+      <c r="DU13" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="14" spans="1:279" s="15" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="b">
+      <c r="A14" s="77" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="77"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="55" t="s">
         <v>35</v>
       </c>
@@ -6525,9 +6543,12 @@
       <c r="DR14" s="57"/>
       <c r="DS14" s="57"/>
       <c r="DT14" s="61"/>
+      <c r="DU14" s="45" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="15" spans="1:279" s="18" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="78" t="b">
+      <c r="A15" s="76" t="b">
         <v>1</v>
       </c>
       <c r="B15" s="75" t="s">
@@ -6813,7 +6834,9 @@
       <c r="DR15" s="66"/>
       <c r="DS15" s="66"/>
       <c r="DT15" s="74"/>
-      <c r="DU15" s="8"/>
+      <c r="DU15" s="45" t="s">
+        <v>233</v>
+      </c>
       <c r="DV15" s="8"/>
       <c r="DW15" s="8"/>
       <c r="DX15" s="8"/>

</xml_diff>